<commit_message>
Initial commit with recent updates
</commit_message>
<xml_diff>
--- a/data/itrade_db.xlsx
+++ b/data/itrade_db.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,19 +18,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -46,27 +42,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -84,12 +65,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -452,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,44 +440,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>username</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>full_name</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>password_hash</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>account_number</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>balance</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>password</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
         </is>
       </c>
     </row>
@@ -533,6 +517,7 @@
           <t>scrypt:32768:8:1$q48AEDJEz9BUcMnS$0fa3b6ee13d27042d3a301a6292bfcdf0c3bab40ede4ed6ea229649ac66be44adb06cdbf836def5ac291f2b09ecfca6652a004a894f7261747edb017ef96b4bc</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -565,6 +550,7 @@
           <t>scrypt:32768:8:1$yvCLXTKlapQnsP0p$91c98e614e3930862fa539cacb1703acebd1582100362747fdc184276a5c45c311533cedfeb2028dd264b94ec2508dd8bf76915c4574efdca36b5010b8650097</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -596,6 +582,252 @@
         <is>
           <t>scrypt:32768:8:1$rYel29Xp0A3q1W0y$42543f8a00370693bb74e47c8e1a98acef42e48cd983ae2547d99a4d5745103003617f54b29db25c4d2a300d3dd540bdf24ec672e96aa86bf84e777e174f893a</t>
         </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>6f2233bf-85ce-4223-97f3-01269e253d59</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GeraldM</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>gerald.mandebvu@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$qZuPwWQuA21XZcX1$d935d811f517d97d6bad7e4e0b38c24e83a32775ace507e7d0ddf73d5dd1a6421258f2867c3fbbe0813f97cd561d6fd835e88d48413bd6e28880e1dcb1e9b59c</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ITRADE-62383392</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" s="2" t="n">
+        <v>45790.53937245371</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2fee1543-82cf-46ea-be0a-04de22ec2134</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GeraldM</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>gerald.mandebvu@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$CWPKJ6xf1eQBf5ZO$89df6aab90151394dfc3bb70285b8c4b4702e6f156dc986edaf07e528161361e182f60529eaaaf450d51a9668fd7ec5faac70ab16dffc278beba0b3a2b9699c1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ITRADE-08672923</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" s="2" t="n">
+        <v>45790.54153032407</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>03b237c3-2ee5-4bb0-a0ce-1a6f6be7b082</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GeraldM</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>gerald.mandebvu@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$ZsHvJm4dnJcazpe1$5bcdbddabe83c75b2caacce86dca516d068d8a3a14164c2ccc7bb2a9616941f3ff12991d14ff34900f300f6a14579991ec92b43c705712509ee963f66538058f</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ITRADE-87632507</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" s="2" t="n">
+        <v>45790.5703228125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6b3a07d9-da57-4ef4-8871-836d18c3a4af</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Trappa</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>itradeafrika@gmail.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$uH5N32tA5P0Tq8LS$98373b4feff7477e98eab68e60e449108888d2ecfb6f09c21e2174fb6765fd240e2b7458696ad9dd43f2ee9d03abc72b5b833a838b6600161b8ff9422bc056c9</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ITRADE-73842040</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" s="2" t="n">
+        <v>45790.59525392361</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>af3de60d-791a-478c-a9e1-a0619a15ae9e</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mandebvug</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>gasnmud@gmail.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$XuF5joyC6cpAcNOO$e80744498c1a79c52f52ee09308ccc3aa15381abc48540da451f59c761c01e47575dadf796986dd7091028b3424a5b4b8eabd1bd940bc05237768eb0dec5eb80</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ITRADE-06641304</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" s="2" t="n">
+        <v>45790.69183142361</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>dbb03cbd-ae2a-4448-9aa1-f8bcadb2e352</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mandebvu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>guwopg@gmail.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$P4T0p2sCwTKtMrPs$5613d614a51993e32b6a6bfa3ea49bf383212e5cc475fc6066312a0188cee74f367a01a3fa6e89303a4d373cd3432739a3e54321e3222a8943965d7368c2d1ae</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ITRADE-19121470</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" s="2" t="n">
+        <v>45790.69401304398</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0381b95b-775a-4450-8eb9-02226ac3b757</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mayc</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>maideic@hotmail.com</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$cXWhhHHQdZ1PDfIo$69cbde31b8c67615e9ee8e903a7d9f6b5f5972c9d2b05e510fa8d0d72472a8c5dc7b27251e3d0a96e46492243105e73db1b1103f9957789268e3841f59cc6f1c</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ITRADE-14298908</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" s="2" t="n">
+        <v>45790.74601511218</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +892,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -731,6 +963,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix registration email, update Dockerfile, and improve user feedback
</commit_message>
<xml_diff>
--- a/data/itrade_db.xlsx
+++ b/data/itrade_db.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -827,7 +827,42 @@
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" s="2" t="n">
-        <v>45790.74601511218</v>
+        <v>45790.74601511574</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>c5578616-d725-4cc3-a2f5-4f5b5ce78ac2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mayy</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>gerald.mandebvu@gmail.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$orxKA4edlVvQvpyn$83571dfbe4eee3d19890937bfbacac0b1c7a438aa4607398e299ae711d706781d2a457ac717f1e85a73585601b4a1dc5c072e812fa05b2f4f10184ae4bbc6e70</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ITRADE-25480410</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" s="2" t="n">
+        <v>45790.86667068065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix send_money flow and indentation issues
</commit_message>
<xml_diff>
--- a/data/itrade_db.xlsx
+++ b/data/itrade_db.xlsx
@@ -10,6 +10,11 @@
     <sheet name="Users" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Beneficiaries" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Transactions" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="beneficiaries1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="beneficiaries2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="beneficiaries3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="beneficiaries4" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="beneficiaries5" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -431,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -862,7 +867,42 @@
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" s="2" t="n">
-        <v>45790.86667068065</v>
+        <v>45790.86667068287</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>a2c7e225-47ae-4256-bcda-1a18c32c60c9</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>alfred</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>itradeafrika@gmail.com</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$ncvVMzyie8R8xpL8$e111dab5a8d1ea649637940b64b48b6c747b3569115c502be01430530d71a81c560812cb6c269902a862721d4b122fe64bfcf6132bab456822c9418526802ff1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ITRADE-01743374</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" s="2" t="n">
+        <v>45799.44844412037</v>
       </c>
     </row>
   </sheetData>
@@ -937,7 +977,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -997,6 +1037,487 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>16f2167b-a447-498b-84af-f8ca89695922</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>a2c7e225-47ae-4256-bcda-1a18c32c60c9</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ZAR</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>45799.45966923611</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_number</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>bank_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>bank_account</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>a596f761-9b33-4a11-a421-1cba17f7d4d3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>a2c7e225-47ae-4256-bcda-1a18c32c60c9</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>mash</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>62312033012</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_number</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>bank_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>bank_account</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>109f3828-20a6-4bd1-80af-b6c90346739b</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>a2c7e225-47ae-4256-bcda-1a18c32c60c9</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>mash</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>62310555012</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_number</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>bank_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>bank_account</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>65faebe2-42d0-479f-9e99-9d558d8927b3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>a2c7e225-47ae-4256-bcda-1a18c32c60c9</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>may</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>5130201124</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_number</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>bank_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>bank_account</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>64b54a56-23c8-4b7e-85cb-a4ae866a1ff0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>a2c7e225-47ae-4256-bcda-1a18c32c60c9</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_number</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>bank_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>bank_account</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>b3bb40b5-05f1-4819-9dfb-addc34e76263</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>a2c7e225-47ae-4256-bcda-1a18c32c60c9</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>62131</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix: Use save_sheet instead of undefined save_df
</commit_message>
<xml_diff>
--- a/data/itrade_db.xlsx
+++ b/data/itrade_db.xlsx
@@ -15,6 +15,8 @@
     <sheet name="beneficiaries3" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="beneficiaries4" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="beneficiaries5" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="beneficiaries6" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="LiveRates" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,6 +905,122 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" s="2" t="n">
         <v>45799.44844412037</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>aaa8d0b9-9355-4483-ab48-6c0ade3eee45</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>gaston</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>gasnmud@gmail.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$a63K5vl6SVSjw0qt$f44f5ad329399a057bb7f79d0ae944a39ac95424794f6e666da5117acdee2cee40cefa617b9ee7f3c65545e2ef7ce5135a94aa8ef4fed37c269dfed816ed298f</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ITRADE-28171340</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" s="2" t="n">
+        <v>45800.44039306713</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.881</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BWP</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>13.48</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CNY</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>7.18</v>
       </c>
     </row>
   </sheetData>
@@ -916,7 +1034,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -963,6 +1081,36 @@
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>9d4d8466-2e96-43b3-a2e0-40dcf39823fb</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>aaa8d0b9-9355-4483-ab48-6c0ade3eee45</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>USD</t>
         </is>
       </c>
     </row>
@@ -977,7 +1125,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1071,6 +1219,162 @@
       </c>
       <c r="J2" s="2" t="n">
         <v>45799.45966923611</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>9b295e02-a0d7-428f-9533-b95ed325c1a4</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>aaa8d0b9-9355-4483-ab48-6c0ade3eee45</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ZAR</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>45801.28394535879</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>40b27379-5469-4097-a613-a9004267ae8e</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>aaa8d0b9-9355-4483-ab48-6c0ade3eee45</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>9d4d8466-2e96-43b3-a2e0-40dcf39823fb</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>45</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Transfer</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>45801.30483710648</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>454fdf4d-62ae-46fd-9a75-2b451e94f840</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>aaa8d0b9-9355-4483-ab48-6c0ade3eee45</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ZAR</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>45801.30553695602</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>fcae4e6d-84f2-4bb9-8f1e-48ad94d7bcdb</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>aaa8d0b9-9355-4483-ab48-6c0ade3eee45</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>9d4d8466-2e96-43b3-a2e0-40dcf39823fb</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>90</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Transfer</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>45801.30565335074</v>
       </c>
     </row>
   </sheetData>
@@ -1507,10 +1811,97 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>62131</t>
-        </is>
+      <c r="G2" t="n">
+        <v>62131</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_number</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>bank_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>bank_account</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>e344cb4b-3245-4934-a82a-ed7eee2adf0a</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>aaa8d0b9-9355-4483-ab48-6c0ade3eee45</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Gerald</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>62312033012</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>

</xml_diff>